<commit_message>
dados na planilha fiis
</commit_message>
<xml_diff>
--- a/controle_fiis_exportado.xlsx
+++ b/controle_fiis_exportado.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Aportes" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Proventos" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rendimentos" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,12 +443,52 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>tipo</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>quantidade</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>preco</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>dy_mes</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>dy_ano</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>dy_percentual</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>dv_ano</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>dv_mes</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>data_com</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>data_cadastrado</t>
         </is>
       </c>
     </row>
@@ -457,11 +498,41 @@
           <t>BTCI11</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>11</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PAPEL</t>
+        </is>
       </c>
       <c r="C2" t="n">
-        <v>9.18</v>
+        <v>50</v>
+      </c>
+      <c r="D2" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="F2" t="n">
+        <v>12.27</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>07/08/2025</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>22/07/2025</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -511,7 +582,100 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10/07/2025</t>
+          <t>22/07/2025</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>FII</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>QTDE COTAS</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ULTIMO PREÇO</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>PROVENTOS</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>RENDIMENTO MÊS</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>RENDIMENTO ANO</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>DATA COM</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>DATA QUE FOI GERADA</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BTCI11</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>50</v>
+      </c>
+      <c r="C2" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>56.00000000000001</v>
+      </c>
+      <c r="F2" t="n">
+        <v>613.5</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>07/08/2025</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>22/07/2025</t>
         </is>
       </c>
     </row>

</xml_diff>